<commit_message>
Day 5 - 11:41am
</commit_message>
<xml_diff>
--- a/pandas/pokemonitems.xlsx
+++ b/pandas/pokemonitems.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -367,65 +367,47 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
+      <c r="A1" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>sacred-ash</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>focus-sash</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>splash-plate</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>fashion-case</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>pikashunium-z--held</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>pikashunium-z--bag</t>
         </is>

</xml_diff>